<commit_message>
edited data and code
</commit_message>
<xml_diff>
--- a/messydata.xlsx
+++ b/messydata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26519"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28020" windowHeight="16100"/>
   </bookViews>
   <sheets>
     <sheet name="1990" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
     <sheet name="2014" sheetId="3" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Titles" localSheetId="0">'1990'!$A:$A,'1990'!#REF!</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">'1990'!#REF!,'1990'!#REF!</definedName>
   </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="29">
   <si>
     <t>Baden-Württemberg</t>
   </si>
@@ -100,6 +100,21 @@
   </si>
   <si>
     <t>winter</t>
+  </si>
+  <si>
+    <t>This is a title we really don't want in our analysis</t>
+  </si>
+  <si>
+    <t>????</t>
+  </si>
+  <si>
+    <t>???</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>Germany</t>
   </si>
 </sst>
 </file>
@@ -214,7 +229,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="67">
+  <cellStyleXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -282,8 +297,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -301,8 +320,21 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="67">
+  <cellStyles count="71">
     <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
@@ -336,6 +368,8 @@
     <cellStyle name="Besuchter Link" xfId="62" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="64" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="70" builtinId="9" hidden="1"/>
     <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
@@ -369,6 +403,8 @@
     <cellStyle name="Link" xfId="61" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="63" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="69" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -698,311 +734,383 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A26" sqref="A26"/>
+      <selection pane="bottomRight" activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="27" customWidth="1"/>
-    <col min="2" max="14" width="11.5" customWidth="1"/>
+    <col min="1" max="3" width="8.83203125" style="8"/>
+    <col min="4" max="4" width="37.33203125" style="8" customWidth="1"/>
+    <col min="5" max="8" width="11.5" style="13" customWidth="1"/>
+    <col min="9" max="11" width="11.5" style="8" customWidth="1"/>
+    <col min="12" max="16384" width="8.83203125" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" thickBot="1">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:8">
+      <c r="A1" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="C2" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="E2" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="F2" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="G2" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="H2" s="12" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15" thickBot="1">
-      <c r="A2" s="2" t="s">
+    <row r="3" spans="1:8">
+      <c r="C3" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="5">
+      <c r="E3" s="12">
         <v>16376</v>
       </c>
-      <c r="C2" s="5">
+      <c r="F3" s="12">
         <v>21321</v>
       </c>
-      <c r="D2" s="5">
+      <c r="G3" s="12">
         <v>15631</v>
       </c>
-      <c r="E2" s="5">
+      <c r="H3" s="12">
         <v>8120</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15" thickBot="1">
-      <c r="A3" s="2" t="s">
+    <row r="4" spans="1:8">
+      <c r="C4" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="5">
+      <c r="E4" s="12">
         <v>19976</v>
       </c>
-      <c r="C3" s="5">
+      <c r="F4" s="12">
         <v>25251</v>
       </c>
-      <c r="D3" s="5">
+      <c r="G4" s="12">
         <v>19071</v>
       </c>
-      <c r="E3" s="5">
+      <c r="H4" s="12">
         <v>10089</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15" thickBot="1">
-      <c r="A4" s="2" t="s">
+    <row r="5" spans="1:8">
+      <c r="C5" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="5">
+      <c r="E5" s="12">
         <v>6194</v>
       </c>
-      <c r="C4" s="5">
+      <c r="F5" s="12">
         <v>7433</v>
       </c>
-      <c r="D4" s="5">
+      <c r="G5" s="12">
         <v>4834</v>
       </c>
-      <c r="E4" s="5">
+      <c r="H5" s="12">
         <v>3389</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15" thickBot="1">
-      <c r="A5" s="2" t="s">
+    <row r="6" spans="1:8">
+      <c r="C6" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="5">
+      <c r="E6" s="12">
         <v>5074</v>
       </c>
-      <c r="C5" s="5">
+      <c r="F6" s="12">
         <v>6680</v>
       </c>
-      <c r="D5" s="5">
+      <c r="G6" s="12">
         <v>3067</v>
       </c>
-      <c r="E5" s="5">
+      <c r="H6" s="12">
         <v>1993</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15" thickBot="1">
-      <c r="A6" s="2" t="s">
+    <row r="7" spans="1:8">
+      <c r="C7" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="5">
+      <c r="E7" s="12">
         <v>1155</v>
       </c>
-      <c r="C6" s="5">
+      <c r="F7" s="12">
         <v>1397</v>
       </c>
-      <c r="D6" s="5">
+      <c r="G7" s="12">
         <v>1061</v>
       </c>
-      <c r="E6" s="5">
+      <c r="H7" s="12">
         <v>725</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15" thickBot="1">
-      <c r="A7" s="2" t="s">
+    <row r="8" spans="1:8">
+      <c r="C8" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="5">
+      <c r="E8" s="12">
         <v>2720</v>
       </c>
-      <c r="C7" s="5">
+      <c r="F8" s="12">
         <v>3152</v>
       </c>
-      <c r="D7" s="5">
+      <c r="G8" s="12">
         <v>2419</v>
       </c>
-      <c r="E7" s="5">
+      <c r="H8" s="12">
         <v>1647</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15" thickBot="1">
-      <c r="A8" s="2" t="s">
+    <row r="9" spans="1:8">
+      <c r="C9" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="5">
+      <c r="E9" s="12">
         <v>9966</v>
       </c>
-      <c r="C8" s="5">
+      <c r="F9" s="12">
         <v>13217</v>
       </c>
-      <c r="D8" s="5">
+      <c r="G9" s="12">
         <v>8298</v>
       </c>
-      <c r="E8" s="5">
+      <c r="H9" s="12">
         <v>5062</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15" thickBot="1">
-      <c r="A9" s="2" t="s">
+    <row r="10" spans="1:8">
+      <c r="C10" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="5">
+      <c r="E10" s="12">
         <v>4177</v>
       </c>
-      <c r="C9" s="5">
+      <c r="F10" s="12">
         <v>4976</v>
       </c>
-      <c r="D9" s="5">
+      <c r="G10" s="12">
         <v>2159</v>
       </c>
-      <c r="E9" s="5">
+      <c r="H10" s="12">
         <v>1394</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15" thickBot="1">
-      <c r="A10" s="2" t="s">
+    <row r="11" spans="1:8">
+      <c r="C11" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="5">
+      <c r="E11" s="12">
         <v>13555</v>
       </c>
-      <c r="C10" s="5">
+      <c r="F11" s="12">
         <v>16780</v>
       </c>
-      <c r="D10" s="5">
+      <c r="G11" s="12">
         <v>11918</v>
       </c>
-      <c r="E10" s="5">
+      <c r="H11" s="12">
         <v>7082</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="15" thickBot="1">
-      <c r="A11" s="2" t="s">
+    <row r="12" spans="1:8">
+      <c r="C12" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="5">
+      <c r="E12" s="12">
         <v>30531</v>
       </c>
-      <c r="C11" s="5">
+      <c r="F12" s="12">
         <v>36184</v>
       </c>
-      <c r="D11" s="5">
+      <c r="G12" s="12">
         <v>28187</v>
       </c>
-      <c r="E11" s="5">
+      <c r="H12" s="12">
         <v>19520</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="15" thickBot="1">
-      <c r="A12" s="2" t="s">
+    <row r="13" spans="1:8">
+      <c r="C13" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="5">
+      <c r="E13" s="12">
         <v>6743</v>
       </c>
-      <c r="C12" s="5">
+      <c r="F13" s="12">
         <v>9394</v>
       </c>
-      <c r="D12" s="5">
+      <c r="G13" s="12">
         <v>5344</v>
       </c>
-      <c r="E12" s="5">
+      <c r="H13" s="12">
         <v>3683</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="15" thickBot="1">
-      <c r="A13" s="2" t="s">
+    <row r="14" spans="1:8">
+      <c r="C14" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="5">
+      <c r="E14" s="12">
         <v>1752</v>
       </c>
-      <c r="C13" s="5">
+      <c r="F14" s="12">
         <v>2602</v>
       </c>
-      <c r="D13" s="5">
+      <c r="G14" s="12">
         <v>1653</v>
       </c>
-      <c r="E13" s="5">
+      <c r="H14" s="12">
         <v>1181</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="15" thickBot="1">
-      <c r="A14" s="2" t="s">
+    <row r="15" spans="1:8">
+      <c r="C15" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="5">
+      <c r="E15" s="12">
         <v>8654</v>
       </c>
-      <c r="C14" s="5">
+      <c r="F15" s="12">
         <v>12169</v>
       </c>
-      <c r="D14" s="5">
+      <c r="G15" s="12">
         <v>5633</v>
       </c>
-      <c r="E14" s="5">
+      <c r="H15" s="12">
         <v>3147</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="15" thickBot="1">
-      <c r="A15" s="2" t="s">
+    <row r="16" spans="1:8">
+      <c r="C16" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="5">
+      <c r="E16" s="12">
         <v>5795</v>
       </c>
-      <c r="C15" s="5">
+      <c r="F16" s="12">
         <v>7238</v>
       </c>
-      <c r="D15" s="5">
+      <c r="G16" s="12">
         <v>3330</v>
       </c>
-      <c r="E15" s="5">
+      <c r="H16" s="12">
         <v>2030</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="15" thickBot="1">
-      <c r="A16" s="2" t="s">
+    <row r="17" spans="3:8">
+      <c r="C17" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="5">
+      <c r="E17" s="12">
         <v>5184</v>
       </c>
-      <c r="C16" s="5">
+      <c r="F17" s="12">
         <v>6565</v>
       </c>
-      <c r="D16" s="5">
+      <c r="G17" s="12">
         <v>4235</v>
       </c>
-      <c r="E16" s="5">
+      <c r="H17" s="12">
         <v>2546</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="15" thickBot="1">
-      <c r="A17" s="3" t="s">
+    <row r="18" spans="3:8">
+      <c r="C18" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D18" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="5">
+      <c r="E18" s="12">
         <v>4757</v>
       </c>
-      <c r="C17" s="5">
+      <c r="F18" s="12">
         <v>5910</v>
       </c>
-      <c r="D17" s="5">
+      <c r="G18" s="12">
         <v>3046</v>
       </c>
-      <c r="E17" s="5">
+      <c r="H18" s="12">
         <v>2016</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="D1:H1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>

</xml_diff>